<commit_message>
Figure and colour scheme tweaks
</commit_message>
<xml_diff>
--- a/lookups/COICOP_maps.xlsx
+++ b/lookups/COICOP_maps.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gamblingcommission-my.sharepoint.com/personal/smurphy_gamblingcommission_gov_uk/Documents/Code/Python/YouGov Finance/Code/gambling-spend-displacement/lookups/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="303" documentId="13_ncr:1_{4EA5ECE4-B677-4D1D-B7A5-75B384F1D133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DF88A695-5054-42C8-8152-9AA5334EB8EF}"/>
+  <xr:revisionPtr revIDLastSave="328" documentId="13_ncr:1_{4EA5ECE4-B677-4D1D-B7A5-75B384F1D133}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{DB0ECA99-418C-424F-9E19-BC4A5DB9A1B1}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -18,7 +18,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">latex!$A$1:$F$34</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lookup!$A$1:$I$34</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">lookup!$A$1:$H$34</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="345" uniqueCount="192">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="321" uniqueCount="171">
   <si>
     <t>code</t>
   </si>
@@ -231,129 +231,6 @@
     <t>Housing &amp; bills</t>
   </si>
   <si>
-    <t>#1f77b4</t>
-  </si>
-  <si>
-    <t>#aec7e8</t>
-  </si>
-  <si>
-    <t>#ff7f0e</t>
-  </si>
-  <si>
-    <t>#ffbb78</t>
-  </si>
-  <si>
-    <t>#2ca02c</t>
-  </si>
-  <si>
-    <t>#98df8a</t>
-  </si>
-  <si>
-    <t>#d62728</t>
-  </si>
-  <si>
-    <t>#ff9896</t>
-  </si>
-  <si>
-    <t>#9467bd</t>
-  </si>
-  <si>
-    <t>#c5b0d5</t>
-  </si>
-  <si>
-    <t>#8c564b</t>
-  </si>
-  <si>
-    <t>#c49c94</t>
-  </si>
-  <si>
-    <t>#e377c2</t>
-  </si>
-  <si>
-    <t>#f7b6d2</t>
-  </si>
-  <si>
-    <t>#7f7f7f</t>
-  </si>
-  <si>
-    <t>#c7c7c7</t>
-  </si>
-  <si>
-    <t>#bcbd22</t>
-  </si>
-  <si>
-    <t>#dbdb8d</t>
-  </si>
-  <si>
-    <t>#17becf</t>
-  </si>
-  <si>
-    <t>#9edae5</t>
-  </si>
-  <si>
-    <t>#92c4e9</t>
-  </si>
-  <si>
-    <t>#0068a9</t>
-  </si>
-  <si>
-    <t>#cda0cb</t>
-  </si>
-  <si>
-    <t>#c23637</t>
-  </si>
-  <si>
-    <t>#f5d77f</t>
-  </si>
-  <si>
-    <t>#c59527</t>
-  </si>
-  <si>
-    <t>#e8c047</t>
-  </si>
-  <si>
-    <t>#f48f3d</t>
-  </si>
-  <si>
-    <t>#d95d5b</t>
-  </si>
-  <si>
-    <t>#b271ab</t>
-  </si>
-  <si>
-    <t>#4d8fcb</t>
-  </si>
-  <si>
-    <t>#912322</t>
-  </si>
-  <si>
-    <t>#ea9a9d</t>
-  </si>
-  <si>
-    <t>#f9c9c7</t>
-  </si>
-  <si>
-    <t>#004586</t>
-  </si>
-  <si>
-    <t>#c1e4f4</t>
-  </si>
-  <si>
-    <t>#926c17</t>
-  </si>
-  <si>
-    <t>#ffefbb</t>
-  </si>
-  <si>
-    <t>#6e2769</t>
-  </si>
-  <si>
-    <t>#e8d0e6</t>
-  </si>
-  <si>
-    <t>nature_rybp</t>
-  </si>
-  <si>
     <t>General purpose retailers</t>
   </si>
   <si>
@@ -376,12 +253,6 @@
   </si>
   <si>
     <t>Donations</t>
-  </si>
-  <si>
-    <t>#d4a6c8</t>
-  </si>
-  <si>
-    <t>#f2c57c</t>
   </si>
   <si>
     <t>COICOP_13.1</t>
@@ -428,9 +299,6 @@
   </si>
   <si>
     <t>Loans</t>
-  </si>
-  <si>
-    <t>#5c6e91</t>
   </si>
   <si>
     <t>Debits to companies identified as loan providers</t>
@@ -625,6 +493,75 @@
   <si>
     <t>Furnishings, household equipment and routine
 household maintenance</t>
+  </si>
+  <si>
+    <t>#3B4992</t>
+  </si>
+  <si>
+    <t>#5F559B</t>
+  </si>
+  <si>
+    <t>#631879</t>
+  </si>
+  <si>
+    <t>#6A4DAE</t>
+  </si>
+  <si>
+    <t>#2C3E8C</t>
+  </si>
+  <si>
+    <t>#1F5AA6</t>
+  </si>
+  <si>
+    <t>#1C7CB6</t>
+  </si>
+  <si>
+    <t>#2A94B3</t>
+  </si>
+  <si>
+    <t>#008280</t>
+  </si>
+  <si>
+    <t>#176D6A</t>
+  </si>
+  <si>
+    <t>#008B45</t>
+  </si>
+  <si>
+    <t>#2E5E3E</t>
+  </si>
+  <si>
+    <t>#A20056</t>
+  </si>
+  <si>
+    <t>#7B2E83</t>
+  </si>
+  <si>
+    <t>#8D2C5B</t>
+  </si>
+  <si>
+    <t>#BB0021</t>
+  </si>
+  <si>
+    <t>#8C1F28</t>
+  </si>
+  <si>
+    <t>#EE0000</t>
+  </si>
+  <si>
+    <t>#B36B00</t>
+  </si>
+  <si>
+    <t>#808180</t>
+  </si>
+  <si>
+    <t>#4A4F57</t>
+  </si>
+  <si>
+    <t>#2A2E34</t>
+  </si>
+  <si>
+    <t>#1B1919</t>
   </si>
 </sst>
 </file>
@@ -738,13 +675,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>386715</xdr:colOff>
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>146685</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>108585</xdr:rowOff>
@@ -806,13 +743,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>9</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>380047</xdr:colOff>
       <xdr:row>7</xdr:row>
       <xdr:rowOff>206692</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>137159</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>92392</xdr:rowOff>
@@ -1245,10 +1182,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J39"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1258,12 +1195,11 @@
     <col min="4" max="4" width="12.59765625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="57.86328125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="23.265625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.46484375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.86328125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.53125" style="6" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.3984375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="15.53125" style="6" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1285,182 +1221,179 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="H1" s="4" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A2" s="3">
         <v>-1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="D2" s="3" t="s">
-        <v>158</v>
+        <v>114</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J2"/>
-    </row>
-    <row r="3" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>87</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I2"/>
+    </row>
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A3" s="3">
         <v>-1.1000000000000001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>152</v>
+        <v>108</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="I3" s="5">
+        <v>104</v>
+      </c>
+      <c r="H3" s="5">
         <v>-1</v>
       </c>
-      <c r="J3"/>
-    </row>
-    <row r="4" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I3"/>
+    </row>
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A4" s="3">
         <v>-1.2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>153</v>
+        <v>109</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>149</v>
-      </c>
-      <c r="I4" s="5">
+        <v>105</v>
+      </c>
+      <c r="H4" s="5">
         <v>-1</v>
       </c>
-      <c r="J4"/>
-    </row>
-    <row r="5" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I4"/>
+    </row>
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A5" s="3">
         <v>-1.3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>144</v>
+        <v>100</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>154</v>
+        <v>110</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>150</v>
-      </c>
-      <c r="I5" s="5">
+        <v>106</v>
+      </c>
+      <c r="H5" s="5">
         <v>-1</v>
       </c>
-      <c r="J5"/>
-    </row>
-    <row r="6" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+      <c r="I5"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A6" s="3">
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>145</v>
+        <v>101</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>157</v>
+        <v>113</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="I6" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J6"/>
-    </row>
-    <row r="7" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+        <v>91</v>
+      </c>
+      <c r="H6" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I6"/>
+    </row>
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A7" s="3">
         <v>0.1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>165</v>
+        <v>121</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>155</v>
+        <v>111</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>136</v>
-      </c>
-      <c r="I7" s="5">
+        <v>92</v>
+      </c>
+      <c r="H7" s="5">
         <v>0</v>
       </c>
-      <c r="J7"/>
-    </row>
-    <row r="8" spans="1:10" s="3" customFormat="1" ht="242.25" x14ac:dyDescent="0.45">
+      <c r="I7"/>
+    </row>
+    <row r="8" spans="1:9" s="3" customFormat="1" ht="242.25" x14ac:dyDescent="0.45">
       <c r="A8" s="3">
         <v>0.2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>166</v>
+        <v>122</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>156</v>
+        <v>112</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="I8" s="5">
+        <v>107</v>
+      </c>
+      <c r="H8" s="5">
         <v>0</v>
       </c>
-      <c r="J8"/>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.45">
+      <c r="I8"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A9">
         <v>1</v>
       </c>
@@ -1468,7 +1401,7 @@
         <v>7</v>
       </c>
       <c r="C9" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D9" t="s">
         <v>29</v>
@@ -1480,16 +1413,13 @@
         <v>51</v>
       </c>
       <c r="G9" t="s">
-        <v>62</v>
-      </c>
-      <c r="H9" t="s">
-        <v>85</v>
-      </c>
-      <c r="I9" s="6">
+        <v>148</v>
+      </c>
+      <c r="H9" s="6">
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A10">
         <v>2</v>
       </c>
@@ -1497,7 +1427,7 @@
         <v>8</v>
       </c>
       <c r="C10" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D10" t="s">
         <v>30</v>
@@ -1509,16 +1439,13 @@
         <v>52</v>
       </c>
       <c r="G10" t="s">
-        <v>63</v>
-      </c>
-      <c r="H10" t="s">
-        <v>86</v>
-      </c>
-      <c r="I10" s="6">
+        <v>149</v>
+      </c>
+      <c r="H10" s="6">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A11">
         <v>3</v>
       </c>
@@ -1526,7 +1453,7 @@
         <v>9</v>
       </c>
       <c r="C11" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D11" t="s">
         <v>31</v>
@@ -1538,16 +1465,13 @@
         <v>53</v>
       </c>
       <c r="G11" t="s">
-        <v>64</v>
-      </c>
-      <c r="H11" t="s">
-        <v>97</v>
-      </c>
-      <c r="I11" s="6">
+        <v>150</v>
+      </c>
+      <c r="H11" s="6">
         <v>3</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A12">
         <v>4</v>
       </c>
@@ -1555,7 +1479,7 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>117</v>
+        <v>74</v>
       </c>
       <c r="D12" t="s">
         <v>32</v>
@@ -1567,16 +1491,13 @@
         <v>61</v>
       </c>
       <c r="G12" t="s">
-        <v>65</v>
-      </c>
-      <c r="H12" t="s">
-        <v>93</v>
-      </c>
-      <c r="I12" s="6">
+        <v>158</v>
+      </c>
+      <c r="H12" s="6">
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
       <c r="A13">
         <v>5</v>
       </c>
@@ -1584,28 +1505,25 @@
         <v>11</v>
       </c>
       <c r="C13" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
       </c>
       <c r="E13" s="10" t="s">
-        <v>191</v>
+        <v>147</v>
       </c>
       <c r="F13" t="s">
         <v>54</v>
       </c>
       <c r="G13" t="s">
-        <v>66</v>
-      </c>
-      <c r="H13" t="s">
-        <v>98</v>
-      </c>
-      <c r="I13" s="6">
+        <v>152</v>
+      </c>
+      <c r="H13" s="6">
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A14">
         <v>6</v>
       </c>
@@ -1613,7 +1531,7 @@
         <v>12</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D14" t="s">
         <v>34</v>
@@ -1625,16 +1543,13 @@
         <v>12</v>
       </c>
       <c r="G14" t="s">
-        <v>67</v>
-      </c>
-      <c r="H14" t="s">
-        <v>88</v>
-      </c>
-      <c r="I14" s="6">
+        <v>153</v>
+      </c>
+      <c r="H14" s="6">
         <v>6</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A15">
         <v>7</v>
       </c>
@@ -1642,7 +1557,7 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>75</v>
       </c>
       <c r="D15" t="s">
         <v>35</v>
@@ -1654,16 +1569,13 @@
         <v>13</v>
       </c>
       <c r="G15" t="s">
-        <v>68</v>
-      </c>
-      <c r="H15" t="s">
-        <v>90</v>
-      </c>
-      <c r="I15" s="6">
+        <v>154</v>
+      </c>
+      <c r="H15" s="6">
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A16">
         <v>8</v>
       </c>
@@ -1671,7 +1583,7 @@
         <v>14</v>
       </c>
       <c r="C16" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D16" t="s">
         <v>36</v>
@@ -1683,16 +1595,13 @@
         <v>55</v>
       </c>
       <c r="G16" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" t="s">
-        <v>92</v>
-      </c>
-      <c r="I16" s="6">
+        <v>151</v>
+      </c>
+      <c r="H16" s="6">
         <v>8</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A17">
         <v>9</v>
       </c>
@@ -1700,7 +1609,7 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
         <v>37</v>
@@ -1712,16 +1621,13 @@
         <v>56</v>
       </c>
       <c r="G17" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" t="s">
-        <v>94</v>
-      </c>
-      <c r="I17" s="6">
+        <v>156</v>
+      </c>
+      <c r="H17" s="6">
         <v>9</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A18">
         <v>10</v>
       </c>
@@ -1729,7 +1635,7 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>120</v>
+        <v>77</v>
       </c>
       <c r="D18" t="s">
         <v>38</v>
@@ -1741,16 +1647,13 @@
         <v>57</v>
       </c>
       <c r="G18" t="s">
-        <v>71</v>
-      </c>
-      <c r="H18" t="s">
-        <v>100</v>
-      </c>
-      <c r="I18" s="6">
+        <v>157</v>
+      </c>
+      <c r="H18" s="6">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A19">
         <v>11</v>
       </c>
@@ -1758,7 +1661,7 @@
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>116</v>
+        <v>73</v>
       </c>
       <c r="D19" t="s">
         <v>39</v>
@@ -1770,40 +1673,37 @@
         <v>58</v>
       </c>
       <c r="G19" t="s">
-        <v>72</v>
-      </c>
-      <c r="H19" t="s">
-        <v>87</v>
-      </c>
-      <c r="I19" s="6">
+        <v>155</v>
+      </c>
+      <c r="H19" s="6">
         <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A20" s="3">
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>139</v>
+        <v>95</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>159</v>
+        <v>115</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="F20" s="3" t="s">
-        <v>162</v>
-      </c>
-      <c r="I20" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J20"/>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.45">
+        <v>118</v>
+      </c>
+      <c r="H20" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I20"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A21">
         <v>12.1</v>
       </c>
@@ -1811,7 +1711,7 @@
         <v>18</v>
       </c>
       <c r="C21" t="s">
-        <v>167</v>
+        <v>123</v>
       </c>
       <c r="D21" t="s">
         <v>40</v>
@@ -1823,69 +1723,63 @@
         <v>18</v>
       </c>
       <c r="G21" t="s">
-        <v>73</v>
-      </c>
-      <c r="H21" t="s">
-        <v>82</v>
-      </c>
-      <c r="I21" s="6">
+        <v>162</v>
+      </c>
+      <c r="H21" s="6">
         <v>12.1</v>
       </c>
     </row>
-    <row r="22" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A22" s="3">
         <v>12.2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>141</v>
+        <v>97</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>161</v>
+        <v>117</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="F22" s="3" t="s">
-        <v>163</v>
-      </c>
-      <c r="I22" s="5" t="s">
-        <v>142</v>
-      </c>
-      <c r="J22"/>
-    </row>
-    <row r="23" spans="1:10" ht="42.75" x14ac:dyDescent="0.45">
+        <v>119</v>
+      </c>
+      <c r="H22" s="5" t="s">
+        <v>98</v>
+      </c>
+      <c r="I22"/>
+    </row>
+    <row r="23" spans="1:9" ht="42.75" x14ac:dyDescent="0.45">
       <c r="A23">
         <v>12.21</v>
       </c>
       <c r="B23" s="10" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="C23" t="s">
-        <v>121</v>
+        <v>78</v>
       </c>
       <c r="D23" t="s">
         <v>41</v>
       </c>
       <c r="E23" s="10" t="s">
-        <v>189</v>
+        <v>145</v>
       </c>
       <c r="F23" t="s">
-        <v>190</v>
+        <v>146</v>
       </c>
       <c r="G23" t="s">
-        <v>76</v>
-      </c>
-      <c r="H23" t="s">
-        <v>84</v>
-      </c>
-      <c r="I23" s="6">
+        <v>160</v>
+      </c>
+      <c r="H23" s="6">
         <v>12.21</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A24">
         <v>12.22</v>
       </c>
@@ -1893,7 +1787,7 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>123</v>
+        <v>80</v>
       </c>
       <c r="D24" t="s">
         <v>42</v>
@@ -1905,16 +1799,13 @@
         <v>20</v>
       </c>
       <c r="G24" t="s">
-        <v>75</v>
-      </c>
-      <c r="H24" t="s">
-        <v>95</v>
-      </c>
-      <c r="I24" s="6">
+        <v>161</v>
+      </c>
+      <c r="H24" s="6">
         <v>12.22</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A25">
         <v>12.23</v>
       </c>
@@ -1922,7 +1813,7 @@
         <v>21</v>
       </c>
       <c r="C25" t="s">
-        <v>124</v>
+        <v>81</v>
       </c>
       <c r="D25" t="s">
         <v>43</v>
@@ -1934,16 +1825,13 @@
         <v>21</v>
       </c>
       <c r="G25" t="s">
-        <v>74</v>
-      </c>
-      <c r="H25" t="s">
-        <v>96</v>
-      </c>
-      <c r="I25" s="6">
+        <v>159</v>
+      </c>
+      <c r="H25" s="6">
         <v>12.23</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A26">
         <v>12.24</v>
       </c>
@@ -1951,7 +1839,7 @@
         <v>22</v>
       </c>
       <c r="C26" t="s">
-        <v>122</v>
+        <v>79</v>
       </c>
       <c r="D26" t="s">
         <v>44</v>
@@ -1963,155 +1851,140 @@
         <v>22</v>
       </c>
       <c r="G26" t="s">
-        <v>77</v>
-      </c>
-      <c r="H26" t="s">
-        <v>101</v>
-      </c>
-      <c r="I26" s="6">
+        <v>163</v>
+      </c>
+      <c r="H26" s="6">
         <v>12.24</v>
       </c>
     </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A27">
         <v>12.25</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="C27" t="s">
-        <v>129</v>
+        <v>85</v>
       </c>
       <c r="D27" t="s">
-        <v>126</v>
+        <v>83</v>
       </c>
       <c r="E27" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="F27" t="s">
-        <v>127</v>
+        <v>84</v>
       </c>
       <c r="G27" t="s">
-        <v>128</v>
-      </c>
-      <c r="H27" t="s">
-        <v>128</v>
-      </c>
-      <c r="I27" s="6">
+        <v>165</v>
+      </c>
+      <c r="H27" s="6">
         <v>12.25</v>
       </c>
     </row>
-    <row r="28" spans="1:10" s="3" customFormat="1" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.45">
       <c r="A28" s="3">
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>146</v>
+        <v>102</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>160</v>
+        <v>116</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="F28" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="I28" s="5">
+        <v>120</v>
+      </c>
+      <c r="H28" s="5">
         <v>13.1</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A29">
         <v>13.1</v>
       </c>
       <c r="B29" t="s">
-        <v>103</v>
+        <v>62</v>
       </c>
       <c r="C29" t="s">
-        <v>106</v>
+        <v>65</v>
       </c>
       <c r="D29" t="s">
-        <v>113</v>
+        <v>70</v>
       </c>
       <c r="E29" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="F29" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="G29" t="s">
-        <v>78</v>
-      </c>
-      <c r="H29" t="s">
-        <v>83</v>
-      </c>
-      <c r="I29" s="6">
+        <v>168</v>
+      </c>
+      <c r="H29" s="6">
         <v>13.1</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A30">
         <v>13.2</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="C30" t="s">
-        <v>107</v>
+        <v>66</v>
       </c>
       <c r="D30" t="s">
-        <v>114</v>
+        <v>71</v>
       </c>
       <c r="E30" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="F30" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="G30" t="s">
-        <v>111</v>
-      </c>
-      <c r="H30" t="s">
-        <v>111</v>
-      </c>
-      <c r="I30" s="6">
+        <v>166</v>
+      </c>
+      <c r="H30" s="6">
         <v>13.2</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A31">
         <v>13.3</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>64</v>
       </c>
       <c r="C31" t="s">
-        <v>108</v>
+        <v>67</v>
       </c>
       <c r="D31" t="s">
-        <v>115</v>
+        <v>72</v>
       </c>
       <c r="E31" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="F31" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="G31" t="s">
-        <v>112</v>
-      </c>
-      <c r="H31" t="s">
-        <v>112</v>
-      </c>
-      <c r="I31" s="6">
+        <v>167</v>
+      </c>
+      <c r="H31" s="6">
         <v>13.3</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.45">
       <c r="A32">
         <v>14</v>
       </c>
@@ -2131,16 +2004,13 @@
         <v>23</v>
       </c>
       <c r="G32" t="s">
-        <v>79</v>
-      </c>
-      <c r="H32" t="s">
-        <v>91</v>
-      </c>
-      <c r="I32" s="6">
+        <v>164</v>
+      </c>
+      <c r="H32" s="6">
         <v>14</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A33">
         <v>15</v>
       </c>
@@ -2160,16 +2030,13 @@
         <v>24</v>
       </c>
       <c r="G33" t="s">
-        <v>80</v>
-      </c>
-      <c r="H33" t="s">
-        <v>99</v>
-      </c>
-      <c r="I33" s="6">
+        <v>169</v>
+      </c>
+      <c r="H33" s="6">
         <v>15</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.45">
       <c r="A34">
         <v>16</v>
       </c>
@@ -2189,20 +2056,17 @@
         <v>59</v>
       </c>
       <c r="G34" t="s">
-        <v>81</v>
-      </c>
-      <c r="H34" t="s">
-        <v>89</v>
-      </c>
-      <c r="I34" s="6">
+        <v>170</v>
+      </c>
+      <c r="H34" s="6">
         <v>16</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.45">
       <c r="B39" s="2"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:I34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
+  <autoFilter ref="A1:H34" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
@@ -2227,19 +2091,19 @@
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
-        <v>168</v>
+        <v>124</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>125</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>129</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>130</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>173</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>174</v>
       </c>
       <c r="F1" s="9" t="str">
         <f>A1 &amp; "  &amp;   " &amp; B1 &amp; "  &amp;   " &amp; C1 &amp; "  &amp;   " &amp; D1 &amp; "  &amp;   " &amp; E1 &amp; "  \\"</f>
@@ -2251,14 +2115,14 @@
         <v>-1</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>131</v>
+        <v>87</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E2" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F2" s="9" t="str">
         <f t="shared" ref="F2:F34" si="0">A2 &amp; "  &amp;   " &amp; B2 &amp; "  &amp;   " &amp; C2 &amp; "  &amp;   " &amp; D2 &amp; "  &amp;   " &amp; E2 &amp; "  \\"</f>
@@ -2270,14 +2134,14 @@
         <v>-1.1000000000000001</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>132</v>
+        <v>88</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F3" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2289,14 +2153,14 @@
         <v>-1.2</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>133</v>
+        <v>89</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F4" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2308,14 +2172,14 @@
         <v>-1.3</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>134</v>
+        <v>90</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E5" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F5" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2327,16 +2191,16 @@
         <v>0</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>135</v>
+        <v>91</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>175</v>
+        <v>131</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F6" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2348,16 +2212,16 @@
         <v>0.1</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>136</v>
+        <v>92</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>176</v>
+        <v>132</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E7" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F7" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2369,16 +2233,16 @@
         <v>0.2</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>137</v>
+        <v>93</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>172</v>
+        <v>128</v>
       </c>
       <c r="D8" s="8" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E8" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F8" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2393,10 +2257,10 @@
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F9" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2411,10 +2275,10 @@
         <v>8</v>
       </c>
       <c r="D10" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F10" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2429,10 +2293,10 @@
         <v>9</v>
       </c>
       <c r="D11" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F11" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2447,13 +2311,13 @@
         <v>10</v>
       </c>
       <c r="C12" t="s">
-        <v>177</v>
+        <v>133</v>
       </c>
       <c r="D12" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F12" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2468,10 +2332,10 @@
         <v>11</v>
       </c>
       <c r="D13" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F13" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2486,10 +2350,10 @@
         <v>12</v>
       </c>
       <c r="D14" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F14" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2504,13 +2368,13 @@
         <v>13</v>
       </c>
       <c r="C15" t="s">
-        <v>178</v>
+        <v>134</v>
       </c>
       <c r="D15" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E15" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F15" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2525,10 +2389,10 @@
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E16" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F16" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2543,13 +2407,13 @@
         <v>15</v>
       </c>
       <c r="C17" t="s">
-        <v>119</v>
+        <v>76</v>
       </c>
       <c r="D17" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E17" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F17" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2564,13 +2428,13 @@
         <v>16</v>
       </c>
       <c r="C18" t="s">
-        <v>179</v>
+        <v>135</v>
       </c>
       <c r="D18" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E18" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F18" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2585,10 +2449,10 @@
         <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E19" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F19" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2600,16 +2464,16 @@
         <v>12</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>138</v>
+        <v>94</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E20" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F20" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2624,10 +2488,10 @@
         <v>18</v>
       </c>
       <c r="D21" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E21" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F21" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2639,16 +2503,16 @@
         <v>12.2</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>140</v>
+        <v>96</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>180</v>
+        <v>136</v>
       </c>
       <c r="D22" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="F22" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2663,13 +2527,13 @@
         <v>19</v>
       </c>
       <c r="C23" t="s">
-        <v>181</v>
+        <v>137</v>
       </c>
       <c r="D23" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E23" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F23" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2684,13 +2548,13 @@
         <v>20</v>
       </c>
       <c r="C24" t="s">
-        <v>182</v>
+        <v>138</v>
       </c>
       <c r="D24" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E24" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F24" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2705,10 +2569,10 @@
         <v>21</v>
       </c>
       <c r="D25" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E25" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F25" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2723,10 +2587,10 @@
         <v>22</v>
       </c>
       <c r="D26" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E26" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F26" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2738,13 +2602,13 @@
         <v>12.25</v>
       </c>
       <c r="B27" t="s">
-        <v>125</v>
+        <v>82</v>
       </c>
       <c r="D27" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E27" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F27" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2756,16 +2620,16 @@
         <v>13</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>147</v>
+        <v>103</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>183</v>
+        <v>139</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="E28" s="5" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F28" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2777,16 +2641,16 @@
         <v>13.1</v>
       </c>
       <c r="B29" t="s">
-        <v>109</v>
+        <v>68</v>
       </c>
       <c r="C29" t="s">
-        <v>188</v>
+        <v>144</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E29" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F29" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2798,13 +2662,13 @@
         <v>13.2</v>
       </c>
       <c r="B30" t="s">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="D30" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E30" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F30" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2816,16 +2680,16 @@
         <v>13.3</v>
       </c>
       <c r="B31" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="C31" t="s">
-        <v>184</v>
+        <v>140</v>
       </c>
       <c r="D31" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E31" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F31" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2840,13 +2704,13 @@
         <v>23</v>
       </c>
       <c r="C32" t="s">
-        <v>185</v>
+        <v>141</v>
       </c>
       <c r="D32" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E32" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F32" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2861,13 +2725,13 @@
         <v>24</v>
       </c>
       <c r="C33" t="s">
-        <v>186</v>
+        <v>142</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F33" s="9" t="str">
         <f t="shared" si="0"/>
@@ -2882,13 +2746,13 @@
         <v>25</v>
       </c>
       <c r="C34" t="s">
-        <v>187</v>
+        <v>143</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>126</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>171</v>
+        <v>127</v>
       </c>
       <c r="F34" s="9" t="str">
         <f t="shared" si="0"/>

</xml_diff>